<commit_message>
naceneni over, 2.5, barvicky
</commit_message>
<xml_diff>
--- a/grantova_zadost_labka__naceneni.xlsx
+++ b/grantova_zadost_labka__naceneni.xlsx
@@ -200,7 +200,7 @@
     <t xml:space="preserve">https://www.alza.cz/macbook-pro-13-retina-cz-2015</t>
   </si>
   <si>
-    <t xml:space="preserve">Dell Latitude E5470 nebo jiné notebooky pro testování</t>
+    <t xml:space="preserve">Dell Latitude E5470 nebo jiné notebooky pro testování – ve stejné cenně víc levnějších</t>
   </si>
   <si>
     <t xml:space="preserve">29496</t>
@@ -400,7 +400,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,14 +415,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -439,8 +451,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -458,7 +482,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE6E6FF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -471,12 +495,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF990000"/>
         <bgColor rgb="FF801900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -685,7 +703,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -802,7 +820,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -814,51 +832,51 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -866,63 +884,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -942,7 +956,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -950,19 +968,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -974,67 +996,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="13" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1046,67 +1068,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="10" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1114,27 +1136,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="16" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="16" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="16" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="16" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1146,11 +1168,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="13" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1190,14 +1212,14 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFE6E6FF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1213,7 +1235,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3399FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1221,7 +1243,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1242,27 +1264,26 @@
   </sheetPr>
   <dimension ref="1:45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C12" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E:E"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="80.3010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.41836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.08163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.28061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.81632653061224"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.95408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.484693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="152.964285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="106.663265306122"/>
-    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="8.97959183673469"/>
-    <col collapsed="false" hidden="false" max="1022" min="975" style="0" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.97959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.71428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.56632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.75510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="163.367346938776"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="113.979591836735"/>
+    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="14.0816326530612"/>
+    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="9.59183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.59183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11407,10 +11428,10 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="35" t="s">
@@ -11425,7 +11446,7 @@
       <c r="F13" s="35" t="n">
         <v>50000</v>
       </c>
-      <c r="G13" s="57" t="n">
+      <c r="G13" s="56" t="n">
         <v>50000</v>
       </c>
       <c r="H13" s="36" t="n">
@@ -11443,7 +11464,7 @@
         <v>21</v>
       </c>
       <c r="L13" s="35"/>
-      <c r="M13" s="58"/>
+      <c r="M13" s="57"/>
       <c r="AKK13" s="42"/>
       <c r="AKL13" s="42"/>
       <c r="AKM13" s="0"/>
@@ -11498,10 +11519,10 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="35" t="s">
@@ -11516,7 +11537,7 @@
       <c r="F14" s="35" t="n">
         <v>30000</v>
       </c>
-      <c r="G14" s="57" t="n">
+      <c r="G14" s="56" t="n">
         <v>30000</v>
       </c>
       <c r="H14" s="36" t="n">
@@ -11534,7 +11555,7 @@
         <v>21</v>
       </c>
       <c r="L14" s="35"/>
-      <c r="M14" s="58"/>
+      <c r="M14" s="57"/>
       <c r="AKK14" s="42"/>
       <c r="AKL14" s="42"/>
       <c r="AKM14" s="0"/>
@@ -11589,10 +11610,10 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="55" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="35" t="s">
@@ -11607,7 +11628,7 @@
       <c r="F15" s="35" t="n">
         <v>150000</v>
       </c>
-      <c r="G15" s="57" t="n">
+      <c r="G15" s="56" t="n">
         <v>50000</v>
       </c>
       <c r="H15" s="36" t="n">
@@ -11625,7 +11646,7 @@
         <v>21</v>
       </c>
       <c r="L15" s="35"/>
-      <c r="M15" s="58"/>
+      <c r="M15" s="57"/>
       <c r="AKK15" s="42"/>
       <c r="AKL15" s="42"/>
       <c r="AKM15" s="0"/>
@@ -11680,7 +11701,7 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="58" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -11689,19 +11710,19 @@
       <c r="C16" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="60" t="s">
+      <c r="F16" s="59" t="s">
         <v>44</v>
       </c>
       <c r="G16" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="H16" s="61" t="s">
+      <c r="H16" s="60" t="s">
         <v>45</v>
       </c>
       <c r="I16" s="27" t="n">
@@ -12682,7 +12703,7 @@
       <c r="AKJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="58" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -12691,7 +12712,7 @@
       <c r="C17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="59" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="20" t="n">
@@ -12703,7 +12724,7 @@
       <c r="G17" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="62" t="n">
+      <c r="H17" s="61" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="27" t="n">
@@ -12720,7 +12741,7 @@
       <c r="L17" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="63"/>
+      <c r="M17" s="62"/>
       <c r="N17" s="0"/>
       <c r="O17" s="0"/>
       <c r="P17" s="0"/>
@@ -13682,7 +13703,7 @@
       <c r="AKJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="63" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="30" t="s">
@@ -13704,7 +13725,7 @@
       <c r="G18" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="62" t="n">
+      <c r="H18" s="61" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="27" t="n">
@@ -13721,7 +13742,7 @@
       <c r="L18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="M18" s="62" t="s">
         <v>50</v>
       </c>
       <c r="N18" s="0"/>
@@ -14724,7 +14745,7 @@
       <c r="L19" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M19" s="63"/>
+      <c r="M19" s="62"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
       <c r="P19" s="0"/>
@@ -15725,7 +15746,7 @@
       <c r="L20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="63"/>
+      <c r="M20" s="62"/>
       <c r="N20" s="0"/>
       <c r="O20" s="0"/>
       <c r="P20" s="0"/>
@@ -16696,7 +16717,7 @@
       <c r="C21" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="59" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="20" t="n">
@@ -16705,7 +16726,7 @@
       <c r="F21" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G21" s="59" t="s">
         <v>56</v>
       </c>
       <c r="H21" s="26" t="n">
@@ -16725,7 +16746,7 @@
       <c r="L21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="63" t="s">
+      <c r="M21" s="62" t="s">
         <v>57</v>
       </c>
       <c r="N21" s="0"/>
@@ -17698,10 +17719,10 @@
       <c r="C22" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="59" t="s">
         <v>60</v>
       </c>
       <c r="F22" s="24" t="n">
@@ -17728,7 +17749,7 @@
       <c r="L22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="63" t="s">
+      <c r="M22" s="62" t="s">
         <v>61</v>
       </c>
       <c r="N22" s="0"/>
@@ -18692,7 +18713,7 @@
       <c r="AKJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="66" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -18701,12 +18722,12 @@
       <c r="C23" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="60"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="20"/>
       <c r="F23" s="24" t="n">
         <v>80000</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="59" t="s">
         <v>63</v>
       </c>
       <c r="H23" s="26" t="n">
@@ -18724,7 +18745,7 @@
         <v>21</v>
       </c>
       <c r="L23" s="20"/>
-      <c r="M23" s="63"/>
+      <c r="M23" s="62"/>
       <c r="N23" s="0"/>
       <c r="O23" s="0"/>
       <c r="P23" s="0"/>
@@ -19686,7 +19707,7 @@
       <c r="AKJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="66" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="30" t="s">
@@ -19695,8 +19716,8 @@
       <c r="C24" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="24" t="n">
         <v>350000</v>
       </c>
@@ -19718,7 +19739,7 @@
         <v>21</v>
       </c>
       <c r="L24" s="20"/>
-      <c r="M24" s="63"/>
+      <c r="M24" s="62"/>
       <c r="N24" s="0"/>
       <c r="O24" s="0"/>
       <c r="P24" s="0"/>
@@ -20680,43 +20701,43 @@
       <c r="AKJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="C25" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="69" t="n">
+      <c r="D25" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E25" s="69" t="n">
+      <c r="E25" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F25" s="69" t="n">
+      <c r="F25" s="70" t="n">
         <v>50000</v>
       </c>
-      <c r="G25" s="69" t="n">
+      <c r="G25" s="70" t="n">
         <v>50000</v>
       </c>
-      <c r="H25" s="69" t="n">
+      <c r="H25" s="70" t="n">
         <v>80000</v>
       </c>
-      <c r="I25" s="70" t="n">
+      <c r="I25" s="71" t="n">
         <f aca="false">F25+G25+H25</f>
         <v>180000</v>
       </c>
-      <c r="J25" s="71" t="n">
+      <c r="J25" s="72" t="n">
         <f aca="false">F25+G25+H25</f>
         <v>180000</v>
       </c>
-      <c r="K25" s="68" t="s">
+      <c r="K25" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
+      <c r="L25" s="70"/>
+      <c r="M25" s="70"/>
       <c r="N25" s="0"/>
       <c r="O25" s="0"/>
       <c r="P25" s="0"/>
@@ -21678,38 +21699,38 @@
       <c r="AKJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="74" t="n">
+      <c r="B26" s="74"/>
+      <c r="C26" s="75" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74" t="n">
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75" t="n">
         <f aca="false">SUM(F3:F23)</f>
         <v>1852741</v>
       </c>
-      <c r="G26" s="74" t="n">
+      <c r="G26" s="75" t="n">
         <f aca="false">SUM(G3:G23)</f>
         <v>378636</v>
       </c>
-      <c r="H26" s="74" t="n">
+      <c r="H26" s="75" t="n">
         <f aca="false">SUM(H3:H23)</f>
         <v>458636</v>
       </c>
-      <c r="I26" s="75" t="n">
+      <c r="I26" s="76" t="n">
         <f aca="false">SUM(I3:I25)</f>
         <v>4064393</v>
       </c>
-      <c r="J26" s="76" t="n">
+      <c r="J26" s="77" t="n">
         <f aca="false">SUM(J3:J25)</f>
         <v>4064393</v>
       </c>
-      <c r="K26" s="77"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="77"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="78"/>
       <c r="N26" s="0"/>
       <c r="O26" s="0"/>
       <c r="P26" s="0"/>
@@ -22671,38 +22692,38 @@
       <c r="AKJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="81" t="n">
+      <c r="C27" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81" t="n">
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="81" t="n">
+      <c r="G27" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="H27" s="81" t="n">
+      <c r="H27" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="I27" s="82" t="n">
+      <c r="I27" s="83" t="n">
         <f aca="false">H27+G27+F27</f>
         <v>0</v>
       </c>
-      <c r="J27" s="83" t="n">
+      <c r="J27" s="84" t="n">
         <v>500000</v>
       </c>
-      <c r="K27" s="84"/>
-      <c r="L27" s="85" t="s">
+      <c r="K27" s="85"/>
+      <c r="L27" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="M27" s="86"/>
+      <c r="M27" s="87"/>
       <c r="N27" s="0"/>
       <c r="O27" s="0"/>
       <c r="P27" s="0"/>
@@ -23663,46 +23684,46 @@
       <c r="AKI27" s="0"/>
       <c r="AKJ27" s="0"/>
     </row>
-    <row r="28" s="90" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="87" t="s">
+    <row r="28" s="91" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="69" t="n">
+      <c r="D28" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E28" s="69" t="n">
+      <c r="E28" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="69" t="n">
+      <c r="F28" s="70" t="n">
         <v>5000</v>
       </c>
-      <c r="G28" s="69" t="n">
+      <c r="G28" s="70" t="n">
         <v>5000</v>
       </c>
-      <c r="H28" s="69" t="n">
+      <c r="H28" s="70" t="n">
         <v>5000</v>
       </c>
-      <c r="I28" s="88" t="n">
+      <c r="I28" s="89" t="n">
         <f aca="false">H28+G28+F28</f>
         <v>15000</v>
       </c>
-      <c r="J28" s="89" t="n">
+      <c r="J28" s="90" t="n">
         <f aca="false">H28+G28+F28</f>
         <v>15000</v>
       </c>
-      <c r="K28" s="68" t="s">
+      <c r="K28" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="AKK28" s="91"/>
-      <c r="AKL28" s="91"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="70"/>
+      <c r="AKK28" s="92"/>
+      <c r="AKL28" s="92"/>
       <c r="AKM28" s="0"/>
       <c r="AKN28" s="0"/>
       <c r="AKO28" s="0"/>
@@ -23755,43 +23776,43 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="87" t="s">
+      <c r="A29" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="69" t="n">
+      <c r="D29" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E29" s="69" t="n">
+      <c r="E29" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F29" s="69" t="n">
+      <c r="F29" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="69" t="n">
+      <c r="G29" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H29" s="69" t="n">
+      <c r="H29" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I29" s="88" t="n">
+      <c r="I29" s="89" t="n">
         <f aca="false">H29+G29+F29</f>
         <v>0</v>
       </c>
-      <c r="J29" s="89" t="n">
+      <c r="J29" s="90" t="n">
         <f aca="false">H29+G29+F29</f>
         <v>0</v>
       </c>
-      <c r="K29" s="68" t="s">
+      <c r="K29" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
       <c r="N29" s="0"/>
       <c r="O29" s="0"/>
       <c r="P29" s="0"/>
@@ -24753,43 +24774,43 @@
       <c r="AKJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="68" t="s">
+      <c r="C30" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="69" t="n">
+      <c r="D30" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E30" s="69" t="n">
+      <c r="E30" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="69" t="n">
+      <c r="F30" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="69" t="n">
+      <c r="G30" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H30" s="69" t="n">
+      <c r="H30" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="88" t="n">
+      <c r="I30" s="89" t="n">
         <f aca="false">H30+G30+F30</f>
         <v>0</v>
       </c>
-      <c r="J30" s="89" t="n">
+      <c r="J30" s="90" t="n">
         <f aca="false">H30+G30+F30</f>
         <v>0</v>
       </c>
-      <c r="K30" s="68" t="s">
+      <c r="K30" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="70"/>
       <c r="N30" s="0"/>
       <c r="O30" s="0"/>
       <c r="P30" s="0"/>
@@ -25751,43 +25772,43 @@
       <c r="AKJ30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="87" t="s">
+      <c r="A31" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="67" t="s">
+      <c r="B31" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="68" t="s">
+      <c r="C31" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="69" t="n">
+      <c r="D31" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E31" s="69" t="n">
+      <c r="E31" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F31" s="69" t="n">
+      <c r="F31" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="69" t="n">
+      <c r="G31" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H31" s="69" t="n">
+      <c r="H31" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="88" t="n">
+      <c r="I31" s="89" t="n">
         <f aca="false">H31+G31+F31</f>
         <v>0</v>
       </c>
-      <c r="J31" s="89" t="n">
+      <c r="J31" s="90" t="n">
         <f aca="false">H31+G31+F31</f>
         <v>0</v>
       </c>
-      <c r="K31" s="68" t="s">
+      <c r="K31" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
       <c r="N31" s="0"/>
       <c r="O31" s="0"/>
       <c r="P31" s="0"/>
@@ -26749,43 +26770,43 @@
       <c r="AKJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="68" t="s">
+      <c r="C32" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="69" t="n">
+      <c r="D32" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E32" s="69" t="n">
+      <c r="E32" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="69" t="n">
+      <c r="F32" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="69" t="n">
+      <c r="G32" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H32" s="69" t="n">
+      <c r="H32" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="88" t="n">
+      <c r="I32" s="89" t="n">
         <f aca="false">H32+G32+F32</f>
         <v>0</v>
       </c>
-      <c r="J32" s="89" t="n">
+      <c r="J32" s="90" t="n">
         <f aca="false">H32+G32+F32</f>
         <v>0</v>
       </c>
-      <c r="K32" s="68" t="s">
+      <c r="K32" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="70"/>
       <c r="N32" s="0"/>
       <c r="O32" s="0"/>
       <c r="P32" s="0"/>
@@ -27747,42 +27768,42 @@
       <c r="AKJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="88" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="69" t="n">
+      <c r="C33" s="70" t="n">
         <v>4</v>
       </c>
-      <c r="D33" s="69" t="n">
+      <c r="D33" s="70" t="n">
         <v>17871</v>
       </c>
-      <c r="E33" s="69" t="n">
+      <c r="E33" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="69" t="n">
+      <c r="F33" s="70" t="n">
         <f aca="false">D33*C33</f>
         <v>71484</v>
       </c>
-      <c r="G33" s="69" t="n">
+      <c r="G33" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H33" s="69" t="n">
+      <c r="H33" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="88" t="n">
+      <c r="I33" s="89" t="n">
         <f aca="false">H33+G33+F33</f>
         <v>71484</v>
       </c>
-      <c r="J33" s="89" t="n">
+      <c r="J33" s="90" t="n">
         <f aca="false">H33+G33+F33</f>
         <v>71484</v>
       </c>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
       <c r="N33" s="0"/>
       <c r="O33" s="0"/>
       <c r="P33" s="0"/>
@@ -28744,46 +28765,46 @@
       <c r="AKJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="69" t="n">
+      <c r="C34" s="70" t="n">
         <v>1000</v>
       </c>
-      <c r="D34" s="69" t="n">
+      <c r="D34" s="70" t="n">
         <v>5</v>
       </c>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69" t="n">
+      <c r="E34" s="70"/>
+      <c r="F34" s="70" t="n">
         <f aca="false">D34*C34</f>
         <v>5000</v>
       </c>
-      <c r="G34" s="69" t="n">
+      <c r="G34" s="70" t="n">
         <f aca="false">D34*C34</f>
         <v>5000</v>
       </c>
-      <c r="H34" s="69" t="n">
+      <c r="H34" s="70" t="n">
         <f aca="false">C34*D34</f>
         <v>5000</v>
       </c>
-      <c r="I34" s="88" t="n">
+      <c r="I34" s="89" t="n">
         <f aca="false">H34+G34+F34</f>
         <v>15000</v>
       </c>
-      <c r="J34" s="89" t="n">
+      <c r="J34" s="90" t="n">
         <f aca="false">H34+G34+F34</f>
         <v>15000</v>
       </c>
-      <c r="K34" s="68" t="s">
+      <c r="K34" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="L34" s="68" t="s">
+      <c r="L34" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="M34" s="69"/>
+      <c r="M34" s="70"/>
       <c r="N34" s="0"/>
       <c r="O34" s="0"/>
       <c r="P34" s="0"/>
@@ -29745,45 +29766,45 @@
       <c r="AKJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="94" t="s">
+      <c r="C35" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="69" t="n">
+      <c r="D35" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="E35" s="69" t="n">
+      <c r="E35" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F35" s="69" t="n">
+      <c r="F35" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="69" t="n">
+      <c r="G35" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H35" s="69" t="n">
+      <c r="H35" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I35" s="88" t="n">
+      <c r="I35" s="89" t="n">
         <f aca="false">H35+G35+F35</f>
         <v>0</v>
       </c>
-      <c r="J35" s="89" t="n">
+      <c r="J35" s="90" t="n">
         <f aca="false">H35+G35+F35</f>
         <v>0</v>
       </c>
-      <c r="K35" s="68" t="s">
+      <c r="K35" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="L35" s="68" t="s">
+      <c r="L35" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="M35" s="69"/>
+      <c r="M35" s="70"/>
       <c r="N35" s="0"/>
       <c r="O35" s="0"/>
       <c r="P35" s="0"/>
@@ -30745,45 +30766,45 @@
       <c r="AKJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="92" t="s">
+      <c r="A36" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="93" t="s">
+      <c r="B36" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="95" t="n">
+      <c r="C36" s="96" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="95" t="n">
+      <c r="D36" s="96" t="n">
         <v>33462.81</v>
       </c>
-      <c r="E36" s="95" t="n">
+      <c r="E36" s="96" t="n">
         <v>40490</v>
       </c>
-      <c r="F36" s="95" t="n">
+      <c r="F36" s="96" t="n">
         <v>40490</v>
       </c>
-      <c r="G36" s="69" t="n">
+      <c r="G36" s="70" t="n">
         <v>20000</v>
       </c>
-      <c r="H36" s="69" t="n">
+      <c r="H36" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I36" s="88" t="n">
+      <c r="I36" s="89" t="n">
         <f aca="false">H36+G36+F36</f>
         <v>60490</v>
       </c>
-      <c r="J36" s="89" t="n">
+      <c r="J36" s="90" t="n">
         <f aca="false">H36+G36+F36</f>
         <v>60490</v>
       </c>
-      <c r="K36" s="68" t="s">
+      <c r="K36" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="L36" s="68" t="s">
+      <c r="L36" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="M36" s="96" t="s">
+      <c r="M36" s="97" t="s">
         <v>82</v>
       </c>
       <c r="N36" s="0"/>
@@ -31747,45 +31768,45 @@
       <c r="AKJ36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="93" t="s">
+      <c r="B37" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="95" t="n">
+      <c r="C37" s="96" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="97" t="s">
+      <c r="D37" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="E37" s="97" t="s">
+      <c r="E37" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="97" t="s">
+      <c r="F37" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="G37" s="69" t="n">
+      <c r="G37" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="H37" s="69" t="n">
+      <c r="H37" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="I37" s="88" t="n">
+      <c r="I37" s="89" t="n">
         <f aca="false">H37+G37+F37</f>
         <v>10499</v>
       </c>
-      <c r="J37" s="89" t="n">
+      <c r="J37" s="90" t="n">
         <f aca="false">H37+G37+F37</f>
         <v>10499</v>
       </c>
-      <c r="K37" s="68" t="s">
+      <c r="K37" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="L37" s="68" t="s">
+      <c r="L37" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="98"/>
+      <c r="M37" s="99"/>
       <c r="N37" s="0"/>
       <c r="O37" s="0"/>
       <c r="P37" s="0"/>
@@ -32746,37 +32767,37 @@
       <c r="AKI37" s="0"/>
       <c r="AKJ37" s="0"/>
     </row>
-    <row r="38" s="106" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="99" t="s">
+    <row r="38" s="107" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="100"/>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101" t="n">
+      <c r="B38" s="101"/>
+      <c r="C38" s="102"/>
+      <c r="D38" s="102"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="102" t="n">
         <f aca="false">SUM(F17:F18)</f>
         <v>43280</v>
       </c>
-      <c r="G38" s="101" t="n">
+      <c r="G38" s="102" t="n">
         <f aca="false">SUM(G17:G18)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="101" t="n">
+      <c r="H38" s="102" t="n">
         <f aca="false">SUM(H17:H18)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="102" t="n">
+      <c r="I38" s="103" t="n">
         <f aca="false">SUM(I26:I37)</f>
         <v>4236866</v>
       </c>
-      <c r="J38" s="103" t="n">
+      <c r="J38" s="104" t="n">
         <f aca="false">SUM(J26:J37)</f>
         <v>4736866</v>
       </c>
-      <c r="K38" s="104"/>
-      <c r="L38" s="105"/>
-      <c r="M38" s="104"/>
+      <c r="K38" s="105"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="105"/>
       <c r="AKM38" s="0"/>
       <c r="AKN38" s="0"/>
       <c r="AKO38" s="0"/>
@@ -32829,21 +32850,21 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="107" t="s">
+      <c r="A39" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="108"/>
-      <c r="C39" s="108"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="108"/>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="109"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="108"/>
-      <c r="L39" s="108"/>
-      <c r="M39" s="108"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="110"/>
+      <c r="J39" s="111"/>
+      <c r="K39" s="109"/>
+      <c r="L39" s="109"/>
+      <c r="M39" s="109"/>
       <c r="N39" s="0"/>
       <c r="O39" s="0"/>
       <c r="P39" s="0"/>
@@ -33805,40 +33826,40 @@
       <c r="AKJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="111" t="s">
+      <c r="A40" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="67" t="s">
+      <c r="B40" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="69" t="n">
+      <c r="C40" s="70" t="n">
         <v>100</v>
       </c>
-      <c r="D40" s="112"/>
-      <c r="E40" s="69" t="n">
+      <c r="D40" s="113"/>
+      <c r="E40" s="70" t="n">
         <v>1000</v>
       </c>
-      <c r="F40" s="95" t="n">
+      <c r="F40" s="96" t="n">
         <f aca="false">C40*E40</f>
         <v>100000</v>
       </c>
-      <c r="G40" s="69"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="113" t="n">
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="114" t="n">
         <f aca="false">C40*E40</f>
         <v>100000</v>
       </c>
-      <c r="J40" s="114" t="n">
+      <c r="J40" s="115" t="n">
         <f aca="false">I40</f>
         <v>100000</v>
       </c>
-      <c r="K40" s="68" t="s">
+      <c r="K40" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L40" s="68" t="s">
+      <c r="L40" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M40" s="69"/>
+      <c r="M40" s="70"/>
       <c r="N40" s="0"/>
       <c r="O40" s="0"/>
       <c r="P40" s="0"/>
@@ -34800,40 +34821,40 @@
       <c r="AKJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="115" t="s">
+      <c r="A41" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="69" t="n">
+      <c r="C41" s="70" t="n">
         <v>20</v>
       </c>
-      <c r="D41" s="112"/>
-      <c r="E41" s="69" t="n">
+      <c r="D41" s="113"/>
+      <c r="E41" s="70" t="n">
         <v>700</v>
       </c>
-      <c r="F41" s="95" t="n">
+      <c r="F41" s="96" t="n">
         <f aca="false">C41*E41</f>
         <v>14000</v>
       </c>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="113" t="n">
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="114" t="n">
         <f aca="false">C41*E41</f>
         <v>14000</v>
       </c>
-      <c r="J41" s="114" t="n">
+      <c r="J41" s="115" t="n">
         <f aca="false">I41</f>
         <v>14000</v>
       </c>
-      <c r="K41" s="68" t="s">
+      <c r="K41" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L41" s="68" t="s">
+      <c r="L41" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M41" s="69"/>
+      <c r="M41" s="70"/>
       <c r="N41" s="0"/>
       <c r="O41" s="0"/>
       <c r="P41" s="0"/>
@@ -35795,40 +35816,40 @@
       <c r="AKJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="111" t="s">
+      <c r="A42" s="112" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="69" t="n">
+      <c r="C42" s="70" t="n">
         <v>500</v>
       </c>
-      <c r="D42" s="112"/>
-      <c r="E42" s="69" t="n">
+      <c r="D42" s="113"/>
+      <c r="E42" s="70" t="n">
         <v>1000</v>
       </c>
-      <c r="F42" s="95" t="n">
+      <c r="F42" s="96" t="n">
         <f aca="false">C42*E42</f>
         <v>500000</v>
       </c>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="113" t="n">
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="114" t="n">
         <f aca="false">C42*E42</f>
         <v>500000</v>
       </c>
-      <c r="J42" s="114" t="n">
+      <c r="J42" s="115" t="n">
         <f aca="false">I42</f>
         <v>500000</v>
       </c>
-      <c r="K42" s="68" t="s">
+      <c r="K42" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L42" s="68" t="s">
+      <c r="L42" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="69"/>
+      <c r="M42" s="70"/>
       <c r="N42" s="0"/>
       <c r="O42" s="0"/>
       <c r="P42" s="0"/>
@@ -36790,40 +36811,40 @@
       <c r="AKJ42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="67" t="s">
+      <c r="B43" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="69" t="n">
+      <c r="C43" s="70" t="n">
         <v>400</v>
       </c>
-      <c r="D43" s="112"/>
-      <c r="E43" s="69" t="n">
+      <c r="D43" s="113"/>
+      <c r="E43" s="70" t="n">
         <v>1000</v>
       </c>
-      <c r="F43" s="95" t="n">
+      <c r="F43" s="96" t="n">
         <f aca="false">C43*E43</f>
         <v>400000</v>
       </c>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="113" t="n">
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="114" t="n">
         <f aca="false">C43*E43</f>
         <v>400000</v>
       </c>
-      <c r="J43" s="114" t="n">
+      <c r="J43" s="115" t="n">
         <f aca="false">I43</f>
         <v>400000</v>
       </c>
-      <c r="K43" s="68" t="s">
+      <c r="K43" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L43" s="68" t="s">
+      <c r="L43" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M43" s="69"/>
+      <c r="M43" s="70"/>
       <c r="N43" s="0"/>
       <c r="O43" s="0"/>
       <c r="P43" s="0"/>
@@ -37785,47 +37806,47 @@
       <c r="AKJ43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="69" t="n">
+      <c r="C44" s="70" t="n">
         <v>300</v>
       </c>
-      <c r="D44" s="112"/>
-      <c r="E44" s="69" t="n">
+      <c r="D44" s="113"/>
+      <c r="E44" s="70" t="n">
         <v>1000</v>
       </c>
-      <c r="F44" s="95" t="n">
+      <c r="F44" s="96" t="n">
         <f aca="false">C44*E44</f>
         <v>300000</v>
       </c>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="113" t="n">
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="114" t="n">
         <f aca="false">C44*E44</f>
         <v>300000</v>
       </c>
-      <c r="J44" s="114" t="n">
+      <c r="J44" s="115" t="n">
         <f aca="false">I44</f>
         <v>300000</v>
       </c>
-      <c r="K44" s="68" t="s">
+      <c r="K44" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="L44" s="68" t="s">
+      <c r="L44" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="M44" s="69"/>
+      <c r="M44" s="70"/>
     </row>
     <row r="45" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I45" s="117" t="n">
+      <c r="I45" s="118" t="n">
         <f aca="false">SUM(I38:I44)</f>
         <v>5550866</v>
       </c>
-      <c r="J45" s="118" t="n">
+      <c r="J45" s="119" t="n">
         <f aca="false">SUM(J38:J44)</f>
         <v>6050866</v>
       </c>

</xml_diff>

<commit_message>
naceneni lepe rozepsane po letech
</commit_message>
<xml_diff>
--- a/grantova_zadost_labka__naceneni.xlsx
+++ b/grantova_zadost_labka__naceneni.xlsx
@@ -17,6 +17,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tato čísla jsou spíše spekulativní</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,26 +1287,27 @@
   </sheetPr>
   <dimension ref="1:45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="85.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.71428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.75510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.25"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="163.367346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="113.979591836735"/>
-    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="14.0816326530612"/>
-    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="9.59183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.59183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="91.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.02040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.26020408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.2244897959184"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.1836734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="174.489795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="121.734693877551"/>
+    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="15"/>
+    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="10.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1022" min="975" style="0" width="8.97959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="10.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5288,18 +5312,18 @@
         <v>500000</v>
       </c>
       <c r="G5" s="20" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="H5" s="26" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="I5" s="27" t="n">
         <f aca="false">F5+G5+H5</f>
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="J5" s="18" t="n">
         <f aca="false">F5+G5+H5</f>
-        <v>500000</v>
+        <v>700000</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>21</v>
@@ -6288,15 +6312,17 @@
         <f aca="false">C6*E6</f>
         <v>200000</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="20" t="n">
+        <v>100000</v>
+      </c>
       <c r="H6" s="26"/>
       <c r="I6" s="27" t="n">
         <f aca="false">F6+G6+H6</f>
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="J6" s="18" t="n">
         <f aca="false">F6+G6+H6</f>
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="20"/>
@@ -8270,11 +8296,14 @@
         <v>600</v>
       </c>
       <c r="F8" s="24" t="n">
-        <f aca="false">C8*E8</f>
-        <v>120000</v>
-      </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="26"/>
+        <v>40000</v>
+      </c>
+      <c r="G8" s="24" t="n">
+        <v>40000</v>
+      </c>
+      <c r="H8" s="24" t="n">
+        <v>40000</v>
+      </c>
       <c r="I8" s="27" t="n">
         <f aca="false">F8+G8+H8</f>
         <v>120000</v>
@@ -9261,10 +9290,11 @@
         <v>1000</v>
       </c>
       <c r="F9" s="24" t="n">
-        <f aca="false">C9*E9</f>
-        <v>200000</v>
-      </c>
-      <c r="G9" s="20"/>
+        <v>150000</v>
+      </c>
+      <c r="G9" s="20" t="n">
+        <v>50000</v>
+      </c>
       <c r="H9" s="26"/>
       <c r="I9" s="27" t="n">
         <f aca="false">F9+G9+H9</f>
@@ -21710,23 +21740,23 @@
       <c r="E26" s="75"/>
       <c r="F26" s="75" t="n">
         <f aca="false">SUM(F3:F23)</f>
-        <v>1852741</v>
+        <v>1722741</v>
       </c>
       <c r="G26" s="75" t="n">
         <f aca="false">SUM(G3:G23)</f>
-        <v>378636</v>
+        <v>668636</v>
       </c>
       <c r="H26" s="75" t="n">
         <f aca="false">SUM(H3:H23)</f>
-        <v>458636</v>
+        <v>598636</v>
       </c>
       <c r="I26" s="76" t="n">
         <f aca="false">SUM(I3:I25)</f>
-        <v>4064393</v>
+        <v>4364393</v>
       </c>
       <c r="J26" s="77" t="n">
         <f aca="false">SUM(J3:J25)</f>
-        <v>4064393</v>
+        <v>4364393</v>
       </c>
       <c r="K26" s="78"/>
       <c r="L26" s="79"/>
@@ -23792,7 +23822,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="70" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="G29" s="70" t="n">
         <v>0</v>
@@ -23802,11 +23832,11 @@
       </c>
       <c r="I29" s="89" t="n">
         <f aca="false">H29+G29+F29</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="J29" s="90" t="n">
         <f aca="false">H29+G29+F29</f>
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="K29" s="69" t="s">
         <v>21</v>
@@ -24790,7 +24820,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="70" t="n">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="G30" s="70" t="n">
         <v>0</v>
@@ -24800,11 +24830,11 @@
       </c>
       <c r="I30" s="89" t="n">
         <f aca="false">H30+G30+F30</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="J30" s="90" t="n">
         <f aca="false">H30+G30+F30</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="K30" s="69" t="s">
         <v>21</v>
@@ -26786,7 +26816,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="70" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="G32" s="70" t="n">
         <v>0</v>
@@ -26796,11 +26826,11 @@
       </c>
       <c r="I32" s="89" t="n">
         <f aca="false">H32+G32+F32</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="J32" s="90" t="n">
         <f aca="false">H32+G32+F32</f>
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="K32" s="69" t="s">
         <v>21</v>
@@ -29782,7 +29812,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="70" t="n">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="G35" s="70" t="n">
         <v>0</v>
@@ -29792,11 +29822,11 @@
       </c>
       <c r="I35" s="89" t="n">
         <f aca="false">H35+G35+F35</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="J35" s="90" t="n">
         <f aca="false">H35+G35+F35</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="K35" s="69" t="s">
         <v>16</v>
@@ -32789,11 +32819,11 @@
       </c>
       <c r="I38" s="103" t="n">
         <f aca="false">SUM(I26:I37)</f>
-        <v>4236866</v>
+        <v>5286866</v>
       </c>
       <c r="J38" s="104" t="n">
         <f aca="false">SUM(J26:J37)</f>
-        <v>4736866</v>
+        <v>5786866</v>
       </c>
       <c r="K38" s="105"/>
       <c r="L38" s="106"/>
@@ -37844,11 +37874,11 @@
     <row r="45" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I45" s="118" t="n">
         <f aca="false">SUM(I38:I44)</f>
-        <v>5550866</v>
+        <v>6600866</v>
       </c>
       <c r="J45" s="119" t="n">
         <f aca="false">SUM(J38:J44)</f>
-        <v>6050866</v>
+        <v>7100866</v>
       </c>
     </row>
   </sheetData>
@@ -37856,7 +37886,7 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="M5" r:id="rId1" display="https://arxiv.org/pdf/1511.09249v1.pdf"/>
+    <hyperlink ref="M5" r:id="rId2" display="https://arxiv.org/pdf/1511.09249v1.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37865,5 +37895,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
naceneni v tisknutelne podobe a pdf
</commit_message>
<xml_diff>
--- a/grantova_zadost_labka__naceneni.xlsx
+++ b/grantova_zadost_labka__naceneni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1287,27 +1287,27 @@
   </sheetPr>
   <dimension ref="1:45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="90.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.80612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="172.520408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="120.413265306122"/>
-    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1022" min="975" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="77.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.80102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.11734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.08163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="7.28061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="8.61224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.7959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="184.280612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="128.576530612245"/>
+    <col collapsed="false" hidden="false" max="972" min="14" style="1" width="15.6122448979592"/>
+    <col collapsed="false" hidden="false" max="974" min="973" style="0" width="10.6122448979592"/>
+    <col collapsed="false" hidden="false" max="1022" min="975" style="0" width="9.38775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="10.6122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>